<commit_message>
Fix/change transitions, disable 1st + last cards transition
</commit_message>
<xml_diff>
--- a/src/Components/Projects/UniProjectsData.xlsx
+++ b/src/Components/Projects/UniProjectsData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\_ Personal Projects\portfolio\src\Components\Projects\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\_ Personal Projects\Portfolio Website\portfolio\src\Components\Projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F25F4CB-BA10-413B-A4FF-B45E18635145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60D4BBB9-B6F3-48D9-AE26-610DCE2813A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="65">
   <si>
     <t>Unit Code</t>
   </si>
@@ -55,9 +55,6 @@
     <t xml:space="preserve">https://www.youtube.com/watch?v=sDHTyitWJQs	</t>
   </si>
   <si>
-    <t xml:space="preserve"> Explore the Twitter API and create a Twitter Bot system to automatically reply to users with a requested image. Makes use of Raspberry Pi’s communication hardware  and software capabilities.</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://youtu.be/GYF2BmvP7JA </t>
   </si>
   <si>
@@ -185,6 +182,39 @@
   </si>
   <si>
     <t>Programming an automated vehicle (simulator) to map and navigate to a location, and perform SLAM.</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Key Skills Developed</t>
+  </si>
+  <si>
+    <t>This Website!</t>
+  </si>
+  <si>
+    <t>HTML, CSS, Javascript, ReactJS</t>
+  </si>
+  <si>
+    <t>Explore the Twitter API and create a Twitter Bot system to automatically reply to users with a requested image. Makes use of Raspberry Pi’s communication hardware  and software capabilities.</t>
+  </si>
+  <si>
+    <t>Creativity</t>
+  </si>
+  <si>
+    <t>Working with Hardware</t>
+  </si>
+  <si>
+    <t>Attention to detail, Creativity, Extra effort pays off</t>
+  </si>
+  <si>
+    <t>Software</t>
+  </si>
+  <si>
+    <t>AI</t>
+  </si>
+  <si>
+    <t>Microcontrollers</t>
   </si>
 </sst>
 </file>
@@ -1039,222 +1069,282 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="62.28515625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="62.28515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>10</v>
+      <c r="E9" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" t="s">
+        <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
+    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>22</v>
+      <c r="E10" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G10" t="s">
+        <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>12</v>
+    <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G11" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" t="s">
-        <v>28</v>
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" t="s">
-        <v>40</v>
-      </c>
-      <c r="C9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E9" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" t="s">
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" t="s">
         <v>41</v>
       </c>
-      <c r="C10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="D13" t="s">
         <v>43</v>
       </c>
-      <c r="C11" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" t="s">
-        <v>42</v>
-      </c>
-      <c r="C12" t="s">
-        <v>44</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{18A8DD12-79F7-4664-8578-E4060F198218}"/>
-    <hyperlink ref="E4" r:id="rId2" display="https://youtu.be/GYF2BmvP7JA" xr:uid="{54B1EA96-B252-4AA2-A7C2-B06701911F16}"/>
+    <hyperlink ref="G3" r:id="rId1" xr:uid="{18A8DD12-79F7-4664-8578-E4060F198218}"/>
+    <hyperlink ref="G5" r:id="rId2" display="https://youtu.be/GYF2BmvP7JA" xr:uid="{54B1EA96-B252-4AA2-A7C2-B06701911F16}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>

</xml_diff>